<commit_message>
s7 bit arrays adjustments
</commit_message>
<xml_diff>
--- a/Snap7/src/tags/s7-tags-s1-p1.xlsx
+++ b/Snap7/src/tags/s7-tags-s1-p1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jbystrzycki\Desktop\Snap7\src\tags\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{800C5C49-761A-4ECE-95C5-2DD8793AB5C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3082D9D-00FF-4020-89BD-4BF4DD798211}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2775" yWindow="2865" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -666,7 +666,7 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E15" sqref="E15"/>
+      <selection pane="bottomRight" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -760,10 +760,10 @@
         <v>100</v>
       </c>
       <c r="E5" s="3">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G5" s="3">
         <v>2</v>
@@ -780,19 +780,19 @@
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D6" s="1">
         <v>100</v>
       </c>
       <c r="E6" s="1">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G6" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H6" s="2"/>
       <c r="I6" s="1"/>
@@ -806,16 +806,16 @@
         <v>7</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D7" s="3">
         <v>100</v>
       </c>
       <c r="E7" s="3">
-        <v>78</v>
+        <v>8</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G7" s="3">
         <v>2</v>

</xml_diff>